<commit_message>
fix: Admin UI improvements, optimize scraper update logic, fix profile match counting bug
</commit_message>
<xml_diff>
--- a/GODOS_ID.xlsx
+++ b/GODOS_ID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mustafa.cevik\Desktop\Kişisel\AOE2DE_GODO_TAKIP_V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC3BED3-E917-4C47-BE3C-59E0C674116D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DAAE88-A849-4271-B31A-755B457B5F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>